<commit_message>
Servo/ flashlight added with desktop app
</commit_message>
<xml_diff>
--- a/pin_config.xlsx
+++ b/pin_config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tamal\Documents\7th_sem\sem_project\application\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB037B4C-D9C2-4A5F-A52B-FA1A62C59010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ACCA758-14DA-4E88-A18C-D1636B3939E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -194,7 +194,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -205,7 +205,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -214,25 +214,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
@@ -518,7 +512,7 @@
   <dimension ref="B1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -554,16 +548,16 @@
         <v>5</v>
       </c>
       <c r="I2" s="10"/>
-      <c r="J2" s="11" t="s">
+      <c r="J2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="K2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="L2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="13" t="s">
+      <c r="M2" s="12" t="s">
         <v>13</v>
       </c>
     </row>
@@ -575,7 +569,7 @@
         <v>12</v>
       </c>
       <c r="D3" s="4">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="E3" s="4">
         <v>0</v>
@@ -586,19 +580,19 @@
       <c r="G3" s="8">
         <v>0</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="15">
+      <c r="J3" s="6">
+        <v>4</v>
+      </c>
+      <c r="K3" s="6">
         <v>2</v>
       </c>
-      <c r="K3" s="15">
-        <v>14</v>
-      </c>
-      <c r="L3" s="16" t="s">
+      <c r="L3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="17" t="s">
+      <c r="M3" s="15" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>